<commit_message>
[#82605732] final code records
</commit_message>
<xml_diff>
--- a/doc/githubStats.xlsx
+++ b/doc/githubStats.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Iteration 1</t>
   </si>
@@ -27,15 +27,6 @@
     <t>294628d75d3df8d9e7c6f8eff5775ac62255cbd2</t>
   </si>
   <si>
-    <t>insersions</t>
-  </si>
-  <si>
-    <t>deletions</t>
-  </si>
-  <si>
-    <t>files changed</t>
-  </si>
-  <si>
     <t>fc3832bcc1e0278ada203550a23c8704d8991359</t>
   </si>
   <si>
@@ -45,15 +36,6 @@
     <t>01205b618a6a95373dbec69107e65c1394af04c2</t>
   </si>
   <si>
-    <t>insersions</t>
-  </si>
-  <si>
-    <t>deletions</t>
-  </si>
-  <si>
-    <t>files changed</t>
-  </si>
-  <si>
     <t>602bc20b2c4eaae4e0711c7a0ecf5b4ec5ad2679</t>
   </si>
   <si>
@@ -63,18 +45,6 @@
     <t>cd5523e609097ee8b8d0bd941497804a9ef82995</t>
   </si>
   <si>
-    <t>insersions</t>
-  </si>
-  <si>
-    <t>deletions</t>
-  </si>
-  <si>
-    <t>files changed</t>
-  </si>
-  <si>
-    <t>5fbfbecfb6736681f109867e810ab99d8224d18b</t>
-  </si>
-  <si>
     <t>Iteration 1 Commits</t>
   </si>
   <si>
@@ -94,24 +64,40 @@
   </si>
   <si>
     <t>Iteration 3 Commits</t>
+  </si>
+  <si>
+    <t>Insertions</t>
+  </si>
+  <si>
+    <t>Deletions</t>
+  </si>
+  <si>
+    <t>Files Changed</t>
+  </si>
+  <si>
+    <t>Doge Driven Development</t>
+  </si>
+  <si>
+    <t>Project: Such Podcast</t>
+  </si>
+  <si>
+    <t>Last Updated: 11PM November 24th</t>
+  </si>
+  <si>
+    <t>6e9f42aabd2ccbac049bb9849ecd932733b942e9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF444444"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -134,6 +120,15 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -149,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -164,27 +159,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -214,8 +303,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Chart title</a:t>
+              <a:t>Code</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Records</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -234,7 +328,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -251,24 +345,24 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>insersions</c:v>
+                  <c:v>Insertions</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>deletions</c:v>
+                  <c:v>Deletions</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>files changed</c:v>
+                  <c:v>Files Changed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:f>Sheet1!$B$5:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -301,7 +395,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -315,24 +409,24 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>insersions</c:v>
+                  <c:v>Insertions</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>deletions</c:v>
+                  <c:v>Deletions</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>files changed</c:v>
+                  <c:v>Files Changed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:f>Sheet1!$A$11:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -365,7 +459,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$9</c:f>
+              <c:f>Sheet1!$B$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -382,24 +476,24 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>insersions</c:v>
+                  <c:v>Insertions</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>deletions</c:v>
+                  <c:v>Deletions</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>files changed</c:v>
+                  <c:v>Files Changed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$12</c:f>
+              <c:f>Sheet1!$B$11:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -432,7 +526,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -446,24 +540,24 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>insersions</c:v>
+                  <c:v>Insertions</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>deletions</c:v>
+                  <c:v>Deletions</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>files changed</c:v>
+                  <c:v>Files Changed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$18</c:f>
+              <c:f>Sheet1!$A$17:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -496,7 +590,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$15</c:f>
+              <c:f>Sheet1!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -513,35 +607,35 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>insersions</c:v>
+                  <c:v>Insertions</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>deletions</c:v>
+                  <c:v>Deletions</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>files changed</c:v>
+                  <c:v>Files Changed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$18</c:f>
+              <c:f>Sheet1!$B$17:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22.0</c:v>
+                  <c:v>517.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>283.0</c:v>
+                  <c:v>69.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,11 +661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2114782504"/>
-        <c:axId val="2114785592"/>
+        <c:axId val="2054526504"/>
+        <c:axId val="2054530056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2114782504"/>
+        <c:axId val="2054526504"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -590,7 +684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2114785592"/>
+        <c:crossAx val="2054530056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -598,7 +692,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114785592"/>
+        <c:axId val="2054530056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2114782504"/>
+        <c:crossAx val="2054526504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -674,8 +768,8 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="180975" y="4133851"/>
-    <xdr:ext cx="5076825" cy="3168650"/>
+    <xdr:pos x="20108" y="4108450"/>
+    <xdr:ext cx="5635625" cy="3384549"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -696,15 +790,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>804333</xdr:colOff>
+      <xdr:colOff>770465</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>59266</xdr:rowOff>
+      <xdr:rowOff>169329</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>499532</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>465664</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>16930</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -713,8 +807,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2675466" y="1032933"/>
-          <a:ext cx="3014133" cy="1676400"/>
+          <a:off x="2641598" y="1278462"/>
+          <a:ext cx="3014133" cy="2184401"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -754,7 +848,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> can the command </a:t>
+            <a:t> used the command:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -769,7 +863,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The commit1 was the first github commit of the iteration and commit2 was the last.</a:t>
+            <a:t>The first commit instance for each bar in the gragh is labled as "commit 1" and "commit2" was the last commit ending on Monday night at Midnight.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1110,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1123,79 +1217,91 @@
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="B3" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="26" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="D3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
         <v>544</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="B16" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1">
@@ -1203,82 +1309,95 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>283</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>35</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="A44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>5</v>
+      <c r="A45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A49" s="5" t="s">
-        <v>20</v>
+      <c r="A49" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A50" s="5" t="s">
-        <v>21</v>
+      <c r="A50" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="D3:E3"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[#82605732] Adding updated excel spreadsheet to go with the updated pdf.
</commit_message>
<xml_diff>
--- a/doc/githubStats.xlsx
+++ b/doc/githubStats.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fileshare\smitchem\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="0" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="1485" yWindow="0" windowWidth="25605" windowHeight="15615" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -248,12 +253,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="13"/>
     </xf>
@@ -265,6 +264,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -278,6 +283,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -367,13 +380,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>544.0</c:v>
+                  <c:v>544</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>191.0</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -431,13 +444,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,13 +511,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>340.0</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,13 +575,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -629,13 +642,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>517.0</c:v>
+                  <c:v>517</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,16 +674,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2054526504"/>
-        <c:axId val="2054530056"/>
+        <c:axId val="140186880"/>
+        <c:axId val="140187272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2054526504"/>
+        <c:axId val="140186880"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
@@ -684,7 +698,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2054530056"/>
+        <c:crossAx val="140187272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -692,7 +706,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2054530056"/>
+        <c:axId val="140187272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -726,7 +740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2054526504"/>
+        <c:crossAx val="140186880"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -745,9 +759,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.826058018545055"/>
-          <c:y val="0.367637637479684"/>
-          <c:w val="0.153929473637559"/>
+          <c:x val="0.82605801854505501"/>
+          <c:y val="0.36763763747968398"/>
+          <c:w val="0.15392947363755899"/>
           <c:h val="0.241477916462847"/>
         </c:manualLayout>
       </c:layout>
@@ -759,7 +773,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -863,7 +877,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The first commit instance for each bar in the gragh is labled as "commit 1" and "commit2" was the last commit ending on Monday night at Midnight.</a:t>
+            <a:t>The first commit instance of an iteration is labled as "commit1" and the last commit is labeled "commit2". Our last commit recorded here was Monday night.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -872,7 +886,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Git stat displays how many lines of code has been added, deleted and how many files changes between the two commit points. </a:t>
+            <a:t>Git stat displays how many lines of code have been added and deleted, as well as how many files changes have been made between the two commit points.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1206,47 +1220,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="1:5" ht="26" customHeight="1">
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="D3" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1254,7 +1268,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1262,7 +1276,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1270,12 +1284,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1283,7 +1297,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1291,7 +1305,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1299,12 +1313,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1326,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1320,7 +1334,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1328,12 +1342,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>9</v>
       </c>
@@ -1341,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>10</v>
       </c>
@@ -1349,12 +1363,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1">
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1">
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>10</v>
       </c>
@@ -1362,7 +1376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1">
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>11</v>
       </c>
@@ -1370,12 +1384,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1">
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1">
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -1399,8 +1413,8 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>